<commit_message>
make sure it works
</commit_message>
<xml_diff>
--- a/description.xlsx
+++ b/description.xlsx
@@ -3,17 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">функция вылавливает рандомно слово для перевода</t>
   </si>
@@ -52,6 +53,39 @@
   </si>
   <si>
     <t xml:space="preserve">своя база слов - догружается по кнопке</t>
+  </si>
+  <si>
+    <t>words</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>lang1</t>
+  </si>
+  <si>
+    <t>lang2</t>
+  </si>
+  <si>
+    <t>sector</t>
+  </si>
+  <si>
+    <t>progress</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>words_id</t>
+  </si>
+  <si>
+    <t>percentage</t>
+  </si>
+  <si>
+    <t>дальше:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">добавить кнопу +1 слово на изучение в шаблон game</t>
   </si>
 </sst>
 </file>
@@ -677,4 +711,66 @@
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>